<commit_message>
expandVarAll corrected expandVar modified to accept parameters send by expandVarAll tests added and vignettes updated
</commit_message>
<xml_diff>
--- a/inst/extdata/genericdictionary.xlsx
+++ b/inst/extdata/genericdictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gedeonz/Dev/R Sources/STRAP Common Tasks/sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gedeonz/Dev/R Sources/STRAP-epiuf/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C07DACE-51F7-FB4A-AFB1-215EDD4387D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5406BDF9-BBE4-7B4A-BBAC-7B3795292736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="5420" windowWidth="31280" windowHeight="21600"/>
+    <workbookView xWindow="8020" yWindow="5420" windowWidth="31280" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>generic_name</t>
   </si>
@@ -82,9 +82,6 @@
     <t>character</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>variable</t>
   </si>
   <si>
-    <t>gaction_group</t>
-  </si>
-  <si>
     <t>parameters</t>
   </si>
   <si>
@@ -116,12 +110,33 @@
   </si>
   <si>
     <t>source3</t>
+  </si>
+  <si>
+    <t>expand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vaccs</t>
+  </si>
+  <si>
+    <t>action_group</t>
+  </si>
+  <si>
+    <t>list(pfizer="pfizer", "moderna"="moderna")</t>
+  </si>
+  <si>
+    <t>YESNO</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -469,10 +484,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -510,7 +525,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -533,13 +548,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="e">
         <v>#N/A</v>
@@ -556,13 +571,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="e">
         <v>#N/A</v>
@@ -674,33 +689,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -711,34 +739,44 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="55.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
test for dico base function getAnyDictionaryValue, doc and comments
</commit_message>
<xml_diff>
--- a/inst/extdata/genericdictionary.xlsx
+++ b/inst/extdata/genericdictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gedeonz/Dev/R Sources/STRAP-epiuf/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5406BDF9-BBE4-7B4A-BBAC-7B3795292736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00775AAC-94F1-C442-BA6B-83F7A241A293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="5420" windowWidth="31280" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8020" yWindow="5420" windowWidth="31280" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>generic_name</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Binary variable</t>
   </si>
 </sst>
 </file>
@@ -487,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -602,11 +605,11 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F5" t="e">
-        <v>#N/A</v>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="G5" t="e">
         <v>#N/A</v>
@@ -692,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -743,7 +746,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -776,6 +779,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
   </sheetData>

</xml_diff>